<commit_message>
Add frailty assessment component
</commit_message>
<xml_diff>
--- a/ref/Text Sources.xlsx
+++ b/ref/Text Sources.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\hacks\covid\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\hacks\covid\ref\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B9DEF574-5507-4737-9CBC-F1991FCA0BF5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79BA7629-D31D-43B9-8240-CDAA2471E536}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="8724" xr2:uid="{065429E4-62E6-4CF2-807E-0DBFF776D3F7}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Very Fit</t>
   </si>
@@ -87,6 +87,15 @@
   </si>
   <si>
     <t>Approaching the end of life. This category applies to people with a *life expectancy &lt; 6 months*, who are *not otherwise evidently frail*.</t>
+  </si>
+  <si>
+    <t>Score</t>
+  </si>
+  <si>
+    <t>Group</t>
+  </si>
+  <si>
+    <t>Description</t>
   </si>
 </sst>
 </file>
@@ -438,14 +447,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{119F91B6-16E1-43B2-AE3C-86D24341E328}">
-  <dimension ref="A2:C10"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection sqref="A1:C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>20</v>
+      </c>
+    </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>

</xml_diff>